<commit_message>
Save correct example from run 15
</commit_message>
<xml_diff>
--- a/dataset/dataset_147_copy.xlsx
+++ b/dataset/dataset_147_copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amilas_Windows_VM\Documents\SheetCoPilot\SheetCopilot\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B9395A-2096-41DB-BD9E-C8A0695A5D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B11CA-D92D-46F7-8E39-B1BDB190AA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$147</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="539">
   <si>
     <t>Sheet Name</t>
   </si>
@@ -1643,16 +1643,6 @@
 Create a column chart with Week as the X-axis and Profit as the Y-axis. (Category: Charts)
 Set the chart title as "Sales Trend". (Category: Charts)
 Add data labels to the chart. (Category: Charts)</t>
-  </si>
-  <si>
-    <t>Create a clustered column chart showing the Sales and COGS data for each week in a new sheet. Set the chart title as "Sales &amp; COGS".</t>
-  </si>
-  <si>
-    <t>Create chart (1), Set chart title (1)</t>
-  </si>
-  <si>
-    <t>Create a clustered column chart in a new sheet and include the Sales and COGS data for each week in the chart. (Category: Charts, Entry and manipulation)
-Set the chart title as "Sales &amp; COGS". (Category: Formatting)</t>
   </si>
   <si>
     <t>XYScatterPlot</t>
@@ -1963,7 +1953,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[dataset_149_copy.xlsx]Sheet2!PivotTable1</c:name>
+    <c:name>[dataset_147_copy.xlsx]Sheet2!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2481,7 +2471,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="hongxin li" refreshedDate="45057.904757523153" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="221" xr:uid="{00000000-000A-0000-FFFF-FFFF07000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J148" sheet="Sheet1"/>
+    <worksheetSource ref="A1:J147" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Sheet Name" numFmtId="0">
@@ -5700,10 +5690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M148"/>
+  <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A64" activeCellId="1" sqref="A21:XFD21 A64:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140:XFD140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5753,7 +5743,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
@@ -5767,10 +5757,10 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -5796,7 +5786,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -6021,7 +6011,7 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F9" t="s">
         <v>43</v>
@@ -6171,7 +6161,7 @@
         <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G13" t="s">
         <v>58</v>
@@ -6315,7 +6305,7 @@
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F17" t="s">
         <v>79</v>
@@ -6336,7 +6326,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="M17" t="e">
         <f t="shared" si="0"/>
@@ -6432,7 +6422,7 @@
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F20" t="s">
         <v>87</v>
@@ -6453,7 +6443,7 @@
         <v>2</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="M20" t="e">
         <f t="shared" si="0"/>
@@ -6972,7 +6962,7 @@
         <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E34" t="s">
         <v>135</v>
@@ -7005,7 +6995,7 @@
         <v>134</v>
       </c>
       <c r="D35" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E35" t="s">
         <v>135</v>
@@ -7038,7 +7028,7 @@
         <v>134</v>
       </c>
       <c r="D36" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E36" t="s">
         <v>135</v>
@@ -7071,7 +7061,7 @@
         <v>134</v>
       </c>
       <c r="D37" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E37" t="s">
         <v>135</v>
@@ -9048,7 +9038,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D90" t="s">
         <v>313</v>
@@ -9078,7 +9068,7 @@
         <v>3</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D91" t="s">
         <v>315</v>
@@ -9117,7 +9107,7 @@
         <v>6</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D92" t="s">
         <v>318</v>
@@ -10734,7 +10724,7 @@
         <v>468</v>
       </c>
       <c r="M134" t="e">
-        <f t="shared" ref="M134:M147" si="3">M133+1</f>
+        <f t="shared" ref="M134:M146" si="3">M133+1</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -10935,67 +10925,67 @@
     </row>
     <row r="140" spans="1:13" ht="15" customHeight="1">
       <c r="A140" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="B140">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="D140" t="s">
-        <v>483</v>
+        <v>485</v>
+      </c>
+      <c r="E140" t="s">
+        <v>486</v>
       </c>
       <c r="F140" t="s">
-        <v>28</v>
+        <v>452</v>
       </c>
       <c r="G140" t="s">
-        <v>484</v>
-      </c>
-      <c r="H140">
-        <v>63</v>
-      </c>
-      <c r="I140" t="s">
-        <v>21</v>
-      </c>
-      <c r="J140" t="s">
-        <v>22</v>
+        <v>487</v>
       </c>
       <c r="K140">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L140" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="M140" t="e">
-        <f t="shared" si="3"/>
+        <f>#REF!+1</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="141" spans="1:13" ht="15" customHeight="1">
       <c r="A141" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B141">
+        <v>2</v>
+      </c>
+      <c r="C141" t="s">
+        <v>484</v>
+      </c>
+      <c r="D141" t="s">
+        <v>489</v>
+      </c>
+      <c r="F141" t="s">
+        <v>79</v>
+      </c>
+      <c r="G141" t="s">
+        <v>67</v>
+      </c>
+      <c r="H141">
+        <v>11</v>
+      </c>
+      <c r="I141" t="s">
+        <v>21</v>
+      </c>
+      <c r="J141" t="s">
+        <v>490</v>
+      </c>
+      <c r="K141">
         <v>1</v>
-      </c>
-      <c r="C141" t="s">
-        <v>487</v>
-      </c>
-      <c r="D141" t="s">
-        <v>488</v>
-      </c>
-      <c r="E141" t="s">
-        <v>489</v>
-      </c>
-      <c r="F141" t="s">
-        <v>452</v>
-      </c>
-      <c r="G141" t="s">
-        <v>490</v>
-      </c>
-      <c r="K141">
-        <v>7</v>
       </c>
       <c r="L141" t="s">
         <v>491</v>
@@ -11007,25 +10997,25 @@
     </row>
     <row r="142" spans="1:13" ht="15" customHeight="1">
       <c r="A142" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D142" t="s">
         <v>492</v>
       </c>
       <c r="F142" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="G142" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="H142">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I142" t="s">
         <v>21</v>
@@ -11046,31 +11036,31 @@
     </row>
     <row r="143" spans="1:13" ht="15" customHeight="1">
       <c r="A143" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B143">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C143" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D143" t="s">
         <v>495</v>
       </c>
       <c r="F143" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="G143" t="s">
-        <v>50</v>
+        <v>496</v>
       </c>
       <c r="H143">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I143" t="s">
         <v>21</v>
       </c>
       <c r="J143" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="K143">
         <v>1</v>
@@ -11085,37 +11075,37 @@
     </row>
     <row r="144" spans="1:13" ht="15" customHeight="1">
       <c r="A144" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B144">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D144" t="s">
         <v>498</v>
       </c>
       <c r="F144" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="G144" t="s">
-        <v>499</v>
+        <v>50</v>
       </c>
       <c r="H144">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I144" t="s">
         <v>21</v>
       </c>
       <c r="J144" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="K144">
         <v>1</v>
       </c>
       <c r="L144" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M144" t="e">
         <f t="shared" si="3"/>
@@ -11124,37 +11114,37 @@
     </row>
     <row r="145" spans="1:13" ht="15" customHeight="1">
       <c r="A145" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B145">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D145" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F145" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="G145" t="s">
-        <v>50</v>
+        <v>459</v>
       </c>
       <c r="H145">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I145" t="s">
         <v>21</v>
       </c>
       <c r="J145" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="K145">
         <v>1</v>
       </c>
       <c r="L145" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M145" t="e">
         <f t="shared" si="3"/>
@@ -11163,37 +11153,37 @@
     </row>
     <row r="146" spans="1:13" ht="15" customHeight="1">
       <c r="A146" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B146">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C146" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D146" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F146" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="G146" t="s">
-        <v>459</v>
+        <v>50</v>
       </c>
       <c r="H146">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I146" t="s">
         <v>21</v>
       </c>
       <c r="J146" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="K146">
         <v>1</v>
       </c>
       <c r="L146" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="M146" t="e">
         <f t="shared" si="3"/>
@@ -11202,84 +11192,45 @@
     </row>
     <row r="147" spans="1:13" ht="15" customHeight="1">
       <c r="A147" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B147">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C147" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D147" t="s">
+        <v>504</v>
+      </c>
+      <c r="F147" t="s">
+        <v>452</v>
+      </c>
+      <c r="G147" t="s">
         <v>505</v>
       </c>
-      <c r="F147" t="s">
-        <v>49</v>
-      </c>
-      <c r="G147" t="s">
-        <v>50</v>
-      </c>
       <c r="H147">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="I147" t="s">
         <v>21</v>
       </c>
       <c r="J147" t="s">
-        <v>496</v>
+        <v>22</v>
       </c>
       <c r="K147">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L147" t="s">
         <v>506</v>
       </c>
       <c r="M147" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" ht="15" customHeight="1">
-      <c r="A148" t="s">
-        <v>486</v>
-      </c>
-      <c r="B148">
-        <v>10</v>
-      </c>
-      <c r="C148" t="s">
-        <v>487</v>
-      </c>
-      <c r="D148" t="s">
-        <v>507</v>
-      </c>
-      <c r="F148" t="s">
-        <v>452</v>
-      </c>
-      <c r="G148" t="s">
-        <v>508</v>
-      </c>
-      <c r="H148">
-        <v>61</v>
-      </c>
-      <c r="I148" t="s">
-        <v>21</v>
-      </c>
-      <c r="J148" t="s">
-        <v>22</v>
-      </c>
-      <c r="K148">
-        <v>4</v>
-      </c>
-      <c r="L148" t="s">
-        <v>509</v>
-      </c>
-      <c r="M148" t="e">
         <f>#REF!+1</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J148" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J147" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -11302,10 +11253,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -11382,7 +11333,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -11566,7 +11517,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="4" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B34">
         <v>221</v>
@@ -11574,10 +11525,10 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -11585,47 +11536,47 @@
         <v>452</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="4" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="4" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>